<commit_message>
update data analysis with data augmentation
</commit_message>
<xml_diff>
--- a/simulation_study_new/simParamsSummary.xlsx
+++ b/simulation_study_new/simParamsSummary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ward-c\Documents\Postdoc\multipleDataBCM\simulation_study8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ward-c\Documents\Postdoc\multipleDataBCM\simulation_study_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B46025-B46C-4CCF-B4C9-C7672A6DC046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A23296-1E20-4DE1-BD41-5358B8170E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{172EBA67-DF58-4CEE-BF06-48D6A2384BDC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{172EBA67-DF58-4CEE-BF06-48D6A2384BDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -474,18 +474,18 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.5703125" style="2" customWidth="1"/>
-    <col min="4" max="5" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="16.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.5546875" style="2" customWidth="1"/>
+    <col min="4" max="5" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -515,7 +515,7 @@
       </c>
       <c r="J1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -535,7 +535,7 @@
         <v>0.1</v>
       </c>
       <c r="G2" s="2">
-        <v>1.4999999999999999E-4</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="H2" s="2">
         <v>0.85</v>
@@ -545,7 +545,7 @@
       </c>
       <c r="J2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
@@ -565,7 +565,7 @@
         <v>0.1</v>
       </c>
       <c r="G3" s="2">
-        <v>1.4999999999999999E-4</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="H3" s="2">
         <v>0.15</v>
@@ -575,7 +575,7 @@
       </c>
       <c r="J3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -595,7 +595,7 @@
         <v>0.1</v>
       </c>
       <c r="G4" s="2">
-        <v>1.4999999999999999E-4</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="H4" s="2">
         <v>0.5</v>
@@ -605,11 +605,11 @@
       </c>
       <c r="J4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
@@ -627,9 +627,9 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -646,7 +646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -685,7 +685,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -721,7 +721,7 @@
         <v>364.16666666666669</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -760,7 +760,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -796,7 +796,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -832,7 +832,7 @@
         <v>334.33333333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -868,7 +868,7 @@
         <v>295.66666666666669</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -904,7 +904,7 @@
         <v>296.5</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -940,7 +940,7 @@
         <v>346.66666666666669</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -976,7 +976,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>263.66666666666669</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>0</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>5</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>6</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>7</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>8</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>9</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>10</v>
       </c>
@@ -1212,12 +1212,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>349.14285714285717</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>404.57142857142856</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>3</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>322.42857142857144</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>4</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>336.71428571428572</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>5</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>338.14285714285717</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>6</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>7</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>393.57142857142856</v>
       </c>
     </row>
-    <row r="34" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>8</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>317.42857142857144</v>
       </c>
     </row>
-    <row r="35" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>9</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>293.14285714285717</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>10</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>367.42857142857144</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>3</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>4</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>5</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>6</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>7</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>8</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>9</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>10</v>
       </c>

</xml_diff>